<commit_message>
NGRX store implemented , Date issue fixed
</commit_message>
<xml_diff>
--- a/customer.xlsx
+++ b/customer.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rohan/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rohan/Documents/dev/Assignments/CustomerPortfolioUploader/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5924111-4465-F040-88B5-D99D319C501D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39726C82-A9F8-1E43-863A-BA3585D3A21E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14760" yWindow="3240" windowWidth="23640" windowHeight="18360" xr2:uid="{273B96C3-68DC-A04A-AF87-2D14238C795C}"/>
+    <workbookView xWindow="8840" yWindow="5660" windowWidth="23640" windowHeight="18360" xr2:uid="{273B96C3-68DC-A04A-AF87-2D14238C795C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,8 +80,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="165" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -112,8 +113,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -429,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CF6AFF7-1BF7-6E40-BAD4-2EC003CCFE1A}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -479,8 +481,8 @@
       <c r="E2">
         <v>3</v>
       </c>
-      <c r="F2" s="1">
-        <v>45641</v>
+      <c r="F2" s="2">
+        <v>45667</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -499,8 +501,8 @@
       <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3" s="1">
-        <v>45616</v>
+      <c r="F3" s="2">
+        <v>45668</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -519,8 +521,8 @@
       <c r="E4">
         <v>4</v>
       </c>
-      <c r="F4" s="1">
-        <v>45570</v>
+      <c r="F4" s="2">
+        <v>45669</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -539,8 +541,8 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5" s="1">
-        <v>45547</v>
+      <c r="F5" s="2">
+        <v>45670</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -559,9 +561,54 @@
       <c r="E6">
         <v>5</v>
       </c>
-      <c r="F6" s="1">
-        <v>45534</v>
-      </c>
+      <c r="F6" s="2">
+        <v>45671</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F21" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>